<commit_message>
Actualizacion Historias de usuario
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACION/1.3 Historias de Usuario/G3_MatrizdeMarcodeTrabajoHU_V2.0_8311.xlsx
+++ b/PREGAME/1. ELICITACION/1.3 Historias de Usuario/G3_MatrizdeMarcodeTrabajoHU_V2.0_8311.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AnalisisyDiseño\8311_G3_ADSW\PREGAME\1. ELICITACION\1.3 Historias de Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266BEFD9-F392-41F5-8340-C65BA8D8CD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F626E4A9-7710-4D36-BA1A-EA06354072D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="92">
   <si>
     <t>Matriz de Marco de Trabajo de HU</t>
   </si>
@@ -258,6 +258,64 @@
   </si>
   <si>
     <t>Iniciar Sesión</t>
+  </si>
+  <si>
+    <t>El aplicativo debera permitir que el administrador pueda agregar nuevas categorías</t>
+  </si>
+  <si>
+    <t>El aplicativo debera permitir al administrador observar las categorías registradas</t>
+  </si>
+  <si>
+    <t>El aplicativo debera permitir al administrador la opcion de editar algun campo de categorías.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El aplicativo debera permitir al administrador la opcion de eliminar una categoria. </t>
+  </si>
+  <si>
+    <t>Registrar Categoria</t>
+  </si>
+  <si>
+    <t>Enlistar Categoria</t>
+  </si>
+  <si>
+    <t>Editar Categoria</t>
+  </si>
+  <si>
+    <t>Eliminar Categoria</t>
+  </si>
+  <si>
+    <t>Para agregar categorias</t>
+  </si>
+  <si>
+    <t>Para mostrar al administrador las categorias registradas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para que el administrador puede editar información </t>
+  </si>
+  <si>
+    <t>Poder eliminar categorías no usadas</t>
+  </si>
+  <si>
+    <t>1.- El aplicativo despliega los atributos descritos que el administrador debe llenar para crear una nueva categoria.
+2.- El aplicativo validará que todos los datos solicitados estén llenos.
+3.- El administrador guarda la información al hacer click en el boton "Añadir".</t>
+  </si>
+  <si>
+    <t>1.- El administrador ingresa al sistema.
+2.- Click en la seccion "Categorias".
+3.- El aplicativo enlista toda la información de las categorias registradas.</t>
+  </si>
+  <si>
+    <t>Registrar categorias</t>
+  </si>
+  <si>
+    <t>Enlistar categorias</t>
+  </si>
+  <si>
+    <t>Editar categorias</t>
+  </si>
+  <si>
+    <t>Eliminar categorias</t>
   </si>
 </sst>
 </file>
@@ -737,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -833,56 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -900,6 +908,59 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1240,9 +1301,7 @@
   </sheetPr>
   <dimension ref="B1:O997"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1272,22 +1331,22 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
     </row>
     <row r="4" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="H4" s="4"/>
@@ -1517,120 +1576,224 @@
       </c>
     </row>
     <row r="10" spans="2:15" ht="78" x14ac:dyDescent="0.25">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="70" t="s">
+      <c r="F10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="70" t="s">
+      <c r="G10" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="70" t="s">
+      <c r="H10" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="72">
+      <c r="I10" s="44">
         <v>4</v>
       </c>
-      <c r="J10" s="71">
+      <c r="J10" s="43">
         <v>44960</v>
       </c>
-      <c r="K10" s="72" t="s">
+      <c r="K10" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="72" t="s">
+      <c r="L10" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="M10" s="70" t="s">
+      <c r="M10" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="N10" s="73" t="s">
+      <c r="N10" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="72" t="s">
+      <c r="O10" s="44" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="109.2" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="15">
+        <v>6</v>
+      </c>
+      <c r="J11" s="16">
+        <v>44963</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="78" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="15">
+        <v>3</v>
+      </c>
+      <c r="J12" s="16">
+        <v>44963</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="156" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="15">
+        <v>4</v>
+      </c>
+      <c r="J13" s="16">
+        <v>44963</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="93.6" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
+      <c r="C14" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="15">
+        <v>4</v>
+      </c>
+      <c r="J14" s="16">
+        <v>44963</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="44" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="15" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
@@ -7632,23 +7795,23 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="2:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="62"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="65"/>
     </row>
     <row r="7" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
@@ -7690,15 +7853,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="61" t="s">
+      <c r="E9" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="62"/>
+      <c r="F9" s="65"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="62"/>
+      <c r="I9" s="65"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -7713,17 +7876,17 @@
         <v>15</v>
       </c>
       <c r="D10" s="23"/>
-      <c r="E10" s="63" t="str">
+      <c r="E10" s="67" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,5,0)</f>
         <v>Administrador</v>
       </c>
-      <c r="F10" s="62"/>
+      <c r="F10" s="65"/>
       <c r="G10" s="24"/>
-      <c r="H10" s="63" t="str">
+      <c r="H10" s="67" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,11,0)</f>
         <v>Terminado</v>
       </c>
-      <c r="I10" s="62"/>
+      <c r="I10" s="65"/>
       <c r="J10" s="24"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
@@ -7755,15 +7918,15 @@
         <v>59</v>
       </c>
       <c r="D12" s="23"/>
-      <c r="E12" s="61" t="s">
+      <c r="E12" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="62"/>
+      <c r="F12" s="65"/>
       <c r="G12" s="24"/>
-      <c r="H12" s="61" t="s">
+      <c r="H12" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="62"/>
+      <c r="I12" s="65"/>
       <c r="J12" s="24"/>
       <c r="K12" s="26"/>
       <c r="L12" s="26"/>
@@ -7779,17 +7942,17 @@
         <v>6</v>
       </c>
       <c r="D13" s="23"/>
-      <c r="E13" s="63" t="str">
+      <c r="E13" s="67" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,10,0)</f>
         <v>Alta</v>
       </c>
-      <c r="F13" s="62"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="63" t="str">
+      <c r="H13" s="67" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,7,0)</f>
         <v>Jhonatan Lituma</v>
       </c>
-      <c r="I13" s="62"/>
+      <c r="I13" s="65"/>
       <c r="J13" s="24"/>
       <c r="K13" s="26"/>
       <c r="L13" s="26"/>
@@ -7817,71 +7980,71 @@
     </row>
     <row r="15" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="49" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="68" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,3,0)</f>
         <v>Registrar Productos</v>
       </c>
-      <c r="E15" s="48"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="49" t="s">
         <v>62</v>
       </c>
       <c r="H15" s="68" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,4,0)</f>
         <v>Para agregar nuevos productos al aplicativo</v>
       </c>
-      <c r="I15" s="47"/>
-      <c r="J15" s="48"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="53"/>
       <c r="K15" s="21"/>
-      <c r="L15" s="43" t="s">
+      <c r="L15" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="M15" s="46" t="str">
+      <c r="M15" s="59" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,6,0)</f>
         <v>1.- El aplicativo despliega los atributos descritos que el administrador debe llenar para crear un nuevo producto. 
 2.- El administrador asigna una categoría al producto.
 3.- El aplicativo validará que todos los datos solicitados estén llenos.
 4.- El administrador guarda la información al hacer click en el boton "Añadir".</v>
       </c>
-      <c r="N15" s="47"/>
-      <c r="O15" s="48"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="53"/>
       <c r="P15" s="35"/>
     </row>
     <row r="16" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="51"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="58"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="51"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="58"/>
       <c r="K16" s="21"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="51"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="58"/>
       <c r="P16" s="35"/>
     </row>
     <row r="17" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="34"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="54"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="54"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="55"/>
       <c r="K17" s="21"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="54"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="55"/>
       <c r="P17" s="35"/>
     </row>
     <row r="18" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7903,41 +8066,41 @@
     </row>
     <row r="19" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34"/>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="55" t="str">
+      <c r="D19" s="53"/>
+      <c r="E19" s="69" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,14,0)</f>
         <v>Registrar productos</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="71"/>
       <c r="P19" s="35"/>
     </row>
     <row r="20" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="34"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="60"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="74"/>
       <c r="P20" s="35"/>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7959,63 +8122,63 @@
     </row>
     <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="34"/>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="46" t="str">
+      <c r="D22" s="53"/>
+      <c r="E22" s="59" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,12,0)</f>
         <v>Crear una prueba unitaria para conocer si el registro procedio con normalidad</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="48"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="53"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="65" t="s">
+      <c r="J22" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="48"/>
-      <c r="L22" s="46" t="str">
+      <c r="K22" s="53"/>
+      <c r="L22" s="59" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O16,13,0)</f>
         <v>Sin comentarios</v>
       </c>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="48"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="53"/>
       <c r="P22" s="35"/>
     </row>
     <row r="23" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="34"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="51"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="58"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="51"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="58"/>
       <c r="P23" s="35"/>
     </row>
     <row r="24" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="34"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="55"/>
       <c r="I24" s="21"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="55"/>
       <c r="P24" s="35"/>
     </row>
     <row r="25" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9032,6 +9195,11 @@
     <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:O17"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="C22:D24"/>
@@ -9048,11 +9216,6 @@
     <mergeCell ref="D15:E17"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:J17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:O17"/>
-    <mergeCell ref="E19:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">

</xml_diff>